<commit_message>
Added code to produce clean figures for publication. TODO: remove anomalous and non-physical variable values.
</commit_message>
<xml_diff>
--- a/interventions_and_attributes.xlsx
+++ b/interventions_and_attributes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="88">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -28,13 +28,13 @@
     <t xml:space="preserve">Intervention name (longLabel)</t>
   </si>
   <si>
-    <t xml:space="preserve">Intervention ID</t>
+    <t xml:space="preserve">interventionId</t>
   </si>
   <si>
     <t xml:space="preserve">Attribute name (shortLabel)</t>
   </si>
   <si>
-    <t xml:space="preserve">Attribute ID</t>
+    <t xml:space="preserve">attributeId</t>
   </si>
   <si>
     <t xml:space="preserve">Back end location (ICCA table)</t>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t xml:space="preserve">PtAssessment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCS component</t>
   </si>
   <si>
     <t xml:space="preserve">GCS Motor</t>
@@ -398,8 +395,8 @@
   </sheetPr>
   <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -468,7 +465,7 @@
         <v>1830</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>6847</v>
@@ -479,7 +476,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>8</v>
@@ -488,7 +485,7 @@
         <v>1830</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>6849</v>
@@ -499,7 +496,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>8</v>
@@ -508,7 +505,7 @@
         <v>1830</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>6851</v>
@@ -519,16 +516,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>2098</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>8590</v>
@@ -539,59 +536,59 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>4322</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>16240</v>
       </c>
       <c r="F7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>4790</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>25649</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>2973</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>8049</v>
@@ -602,16 +599,16 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>3231</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>19522</v>
@@ -622,16 +619,16 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>3361</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>12754</v>
@@ -642,16 +639,16 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>7838</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>27308</v>
@@ -662,16 +659,16 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>7838</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>27312</v>
@@ -682,62 +679,62 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>756</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>20763</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>20306</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>16240</v>
       </c>
       <c r="F15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="G15" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>27</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>2199</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>440</v>
@@ -748,16 +745,16 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>2496</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>15702</v>
@@ -768,16 +765,16 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>3451</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>17151</v>
@@ -788,16 +785,16 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>1746</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" s="0" t="n">
         <v>20883</v>
@@ -808,16 +805,16 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>1746</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>20884</v>
@@ -828,16 +825,16 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>7832</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>27385</v>
@@ -848,16 +845,16 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="0" t="n">
         <v>7832</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>27388</v>
@@ -868,16 +865,16 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="0" t="n">
         <v>3931</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E23" s="0" t="n">
         <v>22195</v>
@@ -888,16 +885,16 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>7792</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E24" s="0" t="n">
         <v>27235</v>
@@ -908,16 +905,16 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>7792</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" s="0" t="n">
         <v>27238</v>
@@ -928,16 +925,16 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>3363</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E26" s="0" t="n">
         <v>10660</v>
@@ -948,16 +945,16 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>3363</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E27" s="0" t="n">
         <v>10663</v>
@@ -968,16 +965,16 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>3363</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>10664</v>
@@ -988,16 +985,16 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>7794</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>27260</v>
@@ -1008,16 +1005,16 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>7794</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E30" s="0" t="n">
         <v>27266</v>
@@ -1028,16 +1025,16 @@
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>7794</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E31" s="0" t="n">
         <v>27270</v>
@@ -1048,16 +1045,16 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>7794</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E32" s="0" t="n">
         <v>27264</v>
@@ -1068,16 +1065,16 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C33" s="0" t="n">
         <v>7794</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E33" s="0" t="n">
         <v>27275</v>
@@ -1088,16 +1085,16 @@
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" s="0" t="n">
         <v>7794</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E34" s="0" t="n">
         <v>27272</v>
@@ -1108,16 +1105,16 @@
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="C35" s="0" t="n">
         <v>21039</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E35" s="0" t="n">
         <v>43381</v>
@@ -1128,16 +1125,16 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" s="0" t="n">
         <v>21039</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>43384</v>
@@ -1148,16 +1145,16 @@
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" s="0" t="n">
         <v>21039</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E37" s="0" t="n">
         <v>43386</v>
@@ -1168,16 +1165,16 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>34</v>
       </c>
       <c r="C38" s="0" t="n">
         <v>21039</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>43388</v>
@@ -1188,16 +1185,16 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C39" s="0" t="n">
         <v>21039</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E39" s="0" t="n">
         <v>43389</v>
@@ -1208,16 +1205,16 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40" s="0" t="n">
         <v>21039</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E40" s="0" t="n">
         <v>43392</v>
@@ -1228,16 +1225,16 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="C41" s="0" t="n">
         <v>3468</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E41" s="0" t="n">
         <v>71</v>
@@ -1248,16 +1245,16 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C42" s="0" t="n">
         <v>3468</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E42" s="0" t="n">
         <v>63</v>
@@ -1268,16 +1265,16 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C43" s="0" t="n">
         <v>3468</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E43" s="0" t="n">
         <v>64</v>
@@ -1288,16 +1285,16 @@
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="C44" s="0" t="n">
         <v>7833</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E44" s="0" t="n">
         <v>27352</v>
@@ -1308,16 +1305,16 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C45" s="0" t="n">
         <v>7833</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E45" s="0" t="n">
         <v>27354</v>
@@ -1328,16 +1325,16 @@
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C46" s="0" t="n">
         <v>7833</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E46" s="0" t="n">
         <v>27350</v>
@@ -1348,16 +1345,16 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="C47" s="0" t="n">
         <v>7833</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E47" s="0" t="n">
         <v>27356</v>
@@ -1368,16 +1365,16 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C48" s="0" t="n">
         <v>7833</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E48" s="0" t="n">
         <v>27367</v>
@@ -1388,16 +1385,16 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C49" s="0" t="n">
         <v>7833</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E49" s="0" t="n">
         <v>27363</v>
@@ -1408,16 +1405,16 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B50" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="C50" s="0" t="n">
         <v>21038</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E50" s="0" t="n">
         <v>43409</v>
@@ -1428,16 +1425,16 @@
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C51" s="0" t="n">
         <v>21038</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E51" s="0" t="n">
         <v>43408</v>
@@ -1448,16 +1445,16 @@
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C52" s="0" t="n">
         <v>21038</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E52" s="0" t="n">
         <v>43399</v>
@@ -1468,16 +1465,16 @@
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="C53" s="0" t="n">
         <v>22287</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E53" s="0" t="n">
         <v>43797</v>
@@ -1488,16 +1485,16 @@
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C54" s="0" t="n">
         <v>22287</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E54" s="0" t="n">
         <v>43800</v>
@@ -1508,16 +1505,16 @@
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C55" s="0" t="n">
         <v>22287</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E55" s="0" t="n">
         <v>43802</v>
@@ -1528,16 +1525,16 @@
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B56" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>41</v>
       </c>
       <c r="C56" s="0" t="n">
         <v>22287</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E56" s="0" t="n">
         <v>43801</v>
@@ -1548,16 +1545,16 @@
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C57" s="0" t="n">
         <v>22287</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E57" s="0" t="n">
         <v>43814</v>
@@ -1568,16 +1565,16 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C58" s="0" t="n">
         <v>22287</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E58" s="0" t="n">
         <v>43811</v>
@@ -1588,16 +1585,16 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B59" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="B59" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="C59" s="0" t="n">
         <v>10939</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E59" s="0" t="n">
         <v>34870</v>
@@ -1608,16 +1605,16 @@
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B60" s="0" t="s">
         <v>44</v>
-      </c>
-      <c r="B60" s="0" t="s">
-        <v>45</v>
       </c>
       <c r="C60" s="0" t="n">
         <v>10939</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E60" s="0" t="n">
         <v>34873</v>
@@ -1628,16 +1625,16 @@
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="B61" s="0" t="s">
-        <v>49</v>
       </c>
       <c r="C61" s="0" t="n">
         <v>3208</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E61" s="0" t="n">
         <v>8584</v>
@@ -1648,16 +1645,16 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C62" s="0" t="n">
         <v>3407</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E62" s="0" t="n">
         <v>3566</v>
@@ -1668,16 +1665,16 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C63" s="0" t="n">
         <v>2154</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E63" s="0" t="n">
         <v>14087</v>
@@ -1688,16 +1685,16 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C64" s="0" t="n">
         <v>30101</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E64" s="0" t="n">
         <v>48821</v>
@@ -1708,16 +1705,16 @@
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C65" s="0" t="n">
         <v>8653</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E65" s="0" t="n">
         <v>32685</v>
@@ -1728,16 +1725,16 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C66" s="0" t="n">
         <v>30178</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E66" s="0" t="n">
         <v>48880</v>
@@ -1748,16 +1745,16 @@
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C67" s="0" t="n">
         <v>8655</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E67" s="0" t="n">
         <v>32674</v>
@@ -1768,16 +1765,16 @@
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C68" s="0" t="n">
         <v>2306</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E68" s="0" t="n">
         <v>21424</v>
@@ -1788,16 +1785,16 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C69" s="0" t="n">
         <v>8655</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E69" s="0" t="n">
         <v>32679</v>
@@ -1808,338 +1805,338 @@
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B70" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="B70" s="0" t="s">
-        <v>55</v>
       </c>
       <c r="C70" s="0" t="n">
         <v>730</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E70" s="0" t="n">
         <v>8960</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B71" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="B71" s="0" t="s">
-        <v>55</v>
       </c>
       <c r="C71" s="0" t="n">
         <v>13965</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E71" s="0" t="n">
         <v>37493</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B72" s="0" t="s">
         <v>58</v>
-      </c>
-      <c r="B72" s="0" t="s">
-        <v>59</v>
       </c>
       <c r="C72" s="0" t="n">
         <v>726</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E72" s="0" t="n">
         <v>7868</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G72" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B73" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="B73" s="0" t="s">
-        <v>62</v>
       </c>
       <c r="C73" s="0" t="n">
         <v>725</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E73" s="0" t="n">
         <v>6138</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B74" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="B74" s="0" t="s">
-        <v>65</v>
       </c>
       <c r="C74" s="0" t="n">
         <v>721</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E74" s="0" t="n">
         <v>9668</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B75" s="0" t="s">
         <v>64</v>
-      </c>
-      <c r="B75" s="0" t="s">
-        <v>65</v>
       </c>
       <c r="C75" s="0" t="n">
         <v>48954</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E75" s="0" t="n">
         <v>16240</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G75" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B76" s="0" t="s">
         <v>67</v>
-      </c>
-      <c r="B76" s="0" t="s">
-        <v>68</v>
       </c>
       <c r="C76" s="0" t="n">
         <v>720</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E76" s="0" t="n">
         <v>2880</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G76" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C77" s="0" t="n">
         <v>4328</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E77" s="0" t="n">
         <v>16240</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G77" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C78" s="0" t="n">
         <v>48959</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E78" s="0" t="n">
         <v>16240</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G78" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C79" s="0" t="n">
         <v>48958</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E79" s="0" t="n">
         <v>16240</v>
       </c>
       <c r="F79" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G79" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C80" s="0" t="n">
         <v>706</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E80" s="0" t="n">
         <v>1865</v>
       </c>
       <c r="F80" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G80" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C81" s="0" t="n">
         <v>510</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E81" s="0" t="n">
         <v>20878</v>
       </c>
       <c r="F81" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G81" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="B82" s="0" t="s">
         <v>72</v>
-      </c>
-      <c r="B82" s="0" t="s">
-        <v>73</v>
       </c>
       <c r="C82" s="0" t="n">
         <v>789</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E82" s="0" t="n">
         <v>20789</v>
       </c>
       <c r="F82" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G82" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="B83" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="B83" s="0" t="s">
-        <v>75</v>
       </c>
       <c r="C83" s="0" t="n">
         <v>758</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E83" s="0" t="n">
         <v>12200</v>
       </c>
       <c r="F83" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G83" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C84" s="0" t="n">
         <v>3431</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E84" s="0" t="n">
         <v>5595</v>
@@ -2150,16 +2147,16 @@
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C85" s="0" t="n">
         <v>3036</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E85" s="0" t="n">
         <v>4620</v>
@@ -2170,278 +2167,278 @@
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="B86" s="0" t="s">
         <v>79</v>
-      </c>
-      <c r="B86" s="0" t="s">
-        <v>80</v>
       </c>
       <c r="C86" s="0" t="n">
         <v>48950</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E86" s="0" t="n">
         <v>16240</v>
       </c>
       <c r="F86" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G86" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="G86" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C87" s="0" t="n">
         <v>13963</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E87" s="0" t="n">
         <v>37502</v>
       </c>
       <c r="F87" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G87" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C88" s="0" t="n">
         <v>48968</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E88" s="0" t="n">
         <v>16240</v>
       </c>
       <c r="F88" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G88" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="G88" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C89" s="0" t="n">
         <v>734</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E89" s="0" t="n">
         <v>10592</v>
       </c>
       <c r="F89" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G89" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="B90" s="0" t="s">
         <v>82</v>
-      </c>
-      <c r="B90" s="0" t="s">
-        <v>83</v>
       </c>
       <c r="C90" s="0" t="n">
         <v>48949</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E90" s="0" t="n">
         <v>16240</v>
       </c>
       <c r="F90" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G90" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="G90" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C91" s="0" t="n">
         <v>13966</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E91" s="0" t="n">
         <v>37522</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G91" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C92" s="0" t="n">
         <v>48967</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E92" s="0" t="n">
         <v>16240</v>
       </c>
       <c r="F92" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G92" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="G92" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C93" s="0" t="n">
         <v>732</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E93" s="0" t="n">
         <v>15246</v>
       </c>
       <c r="F93" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G93" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="B94" s="0" t="s">
         <v>86</v>
-      </c>
-      <c r="B94" s="0" t="s">
-        <v>87</v>
       </c>
       <c r="C94" s="0" t="n">
         <v>4651</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E94" s="0" t="n">
         <v>25545</v>
       </c>
       <c r="F94" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G94" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C95" s="0" t="n">
         <v>522</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E95" s="0" t="n">
         <v>7153</v>
       </c>
       <c r="F95" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G95" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C96" s="0" t="n">
         <v>22544</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E96" s="0" t="n">
         <v>43949</v>
       </c>
       <c r="F96" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G96" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C97" s="0" t="n">
         <v>9502</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E97" s="0" t="n">
         <v>16240</v>
       </c>
       <c r="F97" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G97" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="G97" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up interventions tables.
</commit_message>
<xml_diff>
--- a/interventions_and_attributes.xlsx
+++ b/interventions_and_attributes.xlsx
@@ -395,19 +395,19 @@
   </sheetPr>
   <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A98" activeCellId="0" sqref="A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.7773279352227"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.9919028340081"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>